<commit_message>
Bala Added Google sign up test cases
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
+    <sheet name="GoogleSignupData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,22 +20,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>SearchString</t>
   </si>
   <si>
     <t>Sri</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>CreatePassword</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>Birthyear</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Moblienumber</t>
+  </si>
+  <si>
+    <t>currentemail</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>selenium.trainingsridhar@gmail.com</t>
+  </si>
+  <si>
+    <t>123@Pass</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>****@gmail.com</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,13 +126,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -344,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -364,4 +436,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>9876543212</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>